<commit_message>
improved mlat mapping doc
</commit_message>
<xml_diff>
--- a/doc/objects/mlat.xlsx
+++ b/doc/objects/mlat.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1181" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1198" uniqueCount="398">
   <si>
     <t xml:space="preserve">COLID</t>
   </si>
@@ -1106,23 +1106,7 @@
     <t xml:space="preserve">042.X</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">m2nm, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">different values in db</t>
-    </r>
+    <t xml:space="preserve">m2nm, different values in db</t>
   </si>
   <si>
     <t xml:space="preserve">042.Y</t>
@@ -1173,6 +1157,9 @@
     <t xml:space="preserve">020.SIM</t>
   </si>
   <si>
+    <t xml:space="preserve">020.SPI</t>
+  </si>
+  <si>
     <t xml:space="preserve">220.Target Address</t>
   </si>
   <si>
@@ -1192,6 +1179,12 @@
   </si>
   <si>
     <t xml:space="preserve">170.TRE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flag invert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">170.GHO</t>
   </si>
   <si>
     <t xml:space="preserve">170.MAH</t>
@@ -1231,7 +1224,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1259,17 +1252,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1320,7 +1302,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1333,10 +1315,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1345,15 +1323,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1377,10 +1347,10 @@
   <dimension ref="A1:U98"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U2" activeCellId="1" sqref="A74 U2"/>
+      <selection pane="topLeft" activeCell="U2" activeCellId="0" sqref="U2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="44.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.01"/>
@@ -3649,19 +3619,19 @@
   </sheetPr>
   <dimension ref="A1:I98"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A74" activeCellId="0" sqref="A74"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E99" activeCellId="0" sqref="E99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="53.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="47.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="53.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.32"/>
   </cols>
@@ -3676,13 +3646,13 @@
       <c r="C1" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>314</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -3696,7 +3666,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>318</v>
       </c>
       <c r="B2" s="0" t="s">
@@ -3719,7 +3689,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>320</v>
       </c>
       <c r="B3" s="0" t="s">
@@ -3819,7 +3789,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>325</v>
       </c>
       <c r="B8" s="0" t="s">
@@ -3882,7 +3852,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>329</v>
       </c>
       <c r="B11" s="0" t="s">
@@ -3899,7 +3869,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>330</v>
       </c>
       <c r="B12" s="0" t="s">
@@ -3919,7 +3889,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
         <v>331</v>
       </c>
       <c r="B13" s="0" t="s">
@@ -3939,7 +3909,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>333</v>
       </c>
       <c r="B14" s="0" t="s">
@@ -3959,7 +3929,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>334</v>
       </c>
       <c r="B15" s="0" t="s">
@@ -4028,7 +3998,7 @@
       <c r="D18" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="5" t="s">
         <v>337</v>
       </c>
       <c r="F18" s="1" t="s">
@@ -4039,7 +4009,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="4" t="s">
         <v>338</v>
       </c>
       <c r="B19" s="0" t="s">
@@ -4051,7 +4021,7 @@
       <c r="D19" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E19" s="4" t="s">
         <v>339</v>
       </c>
       <c r="F19" s="1" t="s">
@@ -4148,7 +4118,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="4" t="s">
         <v>341</v>
       </c>
       <c r="B24" s="0" t="s">
@@ -4168,7 +4138,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="4" t="s">
         <v>341</v>
       </c>
       <c r="B25" s="0" t="s">
@@ -4265,7 +4235,7 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="4" t="s">
         <v>338</v>
       </c>
       <c r="B30" s="0" t="s">
@@ -4277,7 +4247,7 @@
       <c r="D30" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="E30" s="7" t="s">
+      <c r="E30" s="4" t="s">
         <v>345</v>
       </c>
       <c r="F30" s="1" t="s">
@@ -4297,7 +4267,7 @@
       <c r="D31" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="E31" s="4" t="s">
         <v>346</v>
       </c>
       <c r="F31" s="1" t="s">
@@ -4488,7 +4458,7 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="6" t="s">
+      <c r="A41" s="5" t="s">
         <v>349</v>
       </c>
       <c r="B41" s="0" t="s">
@@ -4628,7 +4598,6 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="8"/>
       <c r="B48" s="0" t="s">
         <v>159</v>
       </c>
@@ -4715,7 +4684,7 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="5" t="s">
+      <c r="A52" s="4" t="s">
         <v>360</v>
       </c>
       <c r="B52" s="0" t="s">
@@ -4758,7 +4727,7 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="5" t="s">
+      <c r="A54" s="4" t="s">
         <v>362</v>
       </c>
       <c r="B54" s="0" t="s">
@@ -4870,7 +4839,7 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="6" t="s">
+      <c r="A59" s="5" t="s">
         <v>365</v>
       </c>
       <c r="B59" s="0" t="s">
@@ -4922,7 +4891,7 @@
       <c r="D61" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="E61" s="5" t="s">
+      <c r="E61" s="4" t="s">
         <v>346</v>
       </c>
       <c r="I61" s="0" t="s">
@@ -4959,7 +4928,7 @@
       <c r="D63" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="E63" s="5" t="s">
+      <c r="E63" s="4" t="s">
         <v>346</v>
       </c>
       <c r="I63" s="0" t="s">
@@ -4980,7 +4949,7 @@
         <v>17</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="I64" s="0" t="s">
         <v>15</v>
@@ -4996,7 +4965,7 @@
       <c r="D65" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="E65" s="5" t="s">
+      <c r="E65" s="4" t="s">
         <v>346</v>
       </c>
       <c r="I65" s="0" t="s">
@@ -5053,7 +5022,7 @@
       <c r="D68" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="E68" s="5" t="s">
+      <c r="E68" s="4" t="s">
         <v>346</v>
       </c>
       <c r="F68" s="1" t="s">
@@ -5073,7 +5042,7 @@
       <c r="D69" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="E69" s="5" t="s">
+      <c r="E69" s="4" t="s">
         <v>346</v>
       </c>
       <c r="F69" s="1" t="s">
@@ -5144,7 +5113,7 @@
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="5" t="s">
+      <c r="A73" s="4" t="s">
         <v>338</v>
       </c>
       <c r="B73" s="0" t="s">
@@ -5156,7 +5125,7 @@
       <c r="D73" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="E73" s="5" t="s">
+      <c r="E73" s="4" t="s">
         <v>345</v>
       </c>
       <c r="F73" s="1" t="s">
@@ -5167,7 +5136,7 @@
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="5" t="s">
+      <c r="A74" s="4" t="s">
         <v>338</v>
       </c>
       <c r="B74" s="0" t="s">
@@ -5179,7 +5148,7 @@
       <c r="D74" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="E74" s="5" t="s">
+      <c r="E74" s="4" t="s">
         <v>345</v>
       </c>
       <c r="F74" s="1" t="s">
@@ -5239,6 +5208,9 @@
       <c r="D77" s="0" t="s">
         <v>21</v>
       </c>
+      <c r="E77" s="0" t="s">
+        <v>358</v>
+      </c>
       <c r="F77" s="1" t="s">
         <v>242</v>
       </c>
@@ -5259,6 +5231,9 @@
       <c r="D78" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="E78" s="0" t="s">
+        <v>326</v>
+      </c>
       <c r="F78" s="1" t="s">
         <v>245</v>
       </c>
@@ -5267,6 +5242,9 @@
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="4" t="s">
+        <v>378</v>
+      </c>
       <c r="B79" s="0" t="s">
         <v>247</v>
       </c>
@@ -5276,6 +5254,9 @@
       <c r="D79" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="E79" s="0" t="s">
+        <v>326</v>
+      </c>
       <c r="F79" s="1" t="s">
         <v>248</v>
       </c>
@@ -5285,7 +5266,7 @@
     </row>
     <row r="80" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B80" s="0" t="s">
         <v>250</v>
@@ -5305,7 +5286,7 @@
     </row>
     <row r="81" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B81" s="0" t="s">
         <v>254</v>
@@ -5316,6 +5297,9 @@
       <c r="D81" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="E81" s="0" t="s">
+        <v>326</v>
+      </c>
       <c r="F81" s="1" t="s">
         <v>255</v>
       </c>
@@ -5325,7 +5309,7 @@
     </row>
     <row r="82" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B82" s="0" t="s">
         <v>257</v>
@@ -5368,7 +5352,7 @@
     </row>
     <row r="84" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="B84" s="0" t="s">
         <v>267</v>
@@ -5388,7 +5372,7 @@
     </row>
     <row r="85" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B85" s="0" t="s">
         <v>271</v>
@@ -5399,6 +5383,9 @@
       <c r="D85" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="E85" s="0" t="s">
+        <v>326</v>
+      </c>
       <c r="F85" s="1" t="s">
         <v>272</v>
       </c>
@@ -5408,7 +5395,7 @@
     </row>
     <row r="86" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B86" s="0" t="s">
         <v>274</v>
@@ -5419,6 +5406,9 @@
       <c r="D86" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="E86" s="0" t="s">
+        <v>326</v>
+      </c>
       <c r="F86" s="1" t="s">
         <v>275</v>
       </c>
@@ -5428,7 +5418,7 @@
     </row>
     <row r="87" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B87" s="0" t="s">
         <v>277</v>
@@ -5439,6 +5429,9 @@
       <c r="D87" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="E87" s="0" t="s">
+        <v>386</v>
+      </c>
       <c r="F87" s="1" t="s">
         <v>278</v>
       </c>
@@ -5447,6 +5440,9 @@
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="s">
+        <v>387</v>
+      </c>
       <c r="B88" s="0" t="s">
         <v>280</v>
       </c>
@@ -5456,6 +5452,9 @@
       <c r="D88" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="E88" s="0" t="s">
+        <v>326</v>
+      </c>
       <c r="F88" s="1" t="s">
         <v>281</v>
       </c>
@@ -5465,7 +5464,7 @@
     </row>
     <row r="89" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="B89" s="0" t="s">
         <v>283</v>
@@ -5476,6 +5475,9 @@
       <c r="D89" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="E89" s="0" t="s">
+        <v>326</v>
+      </c>
       <c r="F89" s="1" t="s">
         <v>284</v>
       </c>
@@ -5485,7 +5487,7 @@
     </row>
     <row r="90" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="B90" s="0" t="s">
         <v>286</v>
@@ -5505,7 +5507,7 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="B91" s="0" t="s">
         <v>289</v>
@@ -5516,13 +5518,16 @@
       <c r="D91" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="E91" s="0" t="s">
+        <v>326</v>
+      </c>
       <c r="I91" s="0" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="B92" s="0" t="s">
         <v>291</v>
@@ -5533,13 +5538,16 @@
       <c r="D92" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="E92" s="0" t="s">
+        <v>326</v>
+      </c>
       <c r="I92" s="0" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="B93" s="0" t="s">
         <v>293</v>
@@ -5550,13 +5558,16 @@
       <c r="D93" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="E93" s="0" t="s">
+        <v>326</v>
+      </c>
       <c r="I93" s="0" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="B94" s="0" t="s">
         <v>295</v>
@@ -5567,13 +5578,16 @@
       <c r="D94" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="E94" s="0" t="s">
+        <v>326</v>
+      </c>
       <c r="I94" s="0" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="B95" s="0" t="s">
         <v>297</v>
@@ -5584,13 +5598,16 @@
       <c r="D95" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="E95" s="0" t="s">
+        <v>326</v>
+      </c>
       <c r="I95" s="0" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="B96" s="0" t="s">
         <v>299</v>
@@ -5601,13 +5618,16 @@
       <c r="D96" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="E96" s="0" t="s">
+        <v>326</v>
+      </c>
       <c r="I96" s="0" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="B97" s="0" t="s">
         <v>301</v>
@@ -5633,7 +5653,7 @@
     </row>
     <row r="98" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="B98" s="0" t="s">
         <v>306</v>

</xml_diff>

<commit_message>
mlat asterix import custom fields
</commit_message>
<xml_diff>
--- a/doc/objects/mlat.xlsx
+++ b/doc/objects/mlat.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1198" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1205" uniqueCount="399">
   <si>
     <t xml:space="preserve">COLID</t>
   </si>
@@ -980,10 +980,10 @@
     <t xml:space="preserve">230.AIC</t>
   </si>
   <si>
-    <t xml:space="preserve">flag Why inverted?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">230.ARC</t>
+    <t xml:space="preserve">flag, inverted in verif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">custom based on 230.ARC</t>
   </si>
   <si>
     <t xml:space="preserve">230.B1A</t>
@@ -1031,7 +1031,7 @@
     <t xml:space="preserve">245.Target Identification</t>
   </si>
   <si>
-    <t xml:space="preserve">custom cat</t>
+    <t xml:space="preserve">custom category</t>
   </si>
   <si>
     <t xml:space="preserve">unknown</t>
@@ -1049,7 +1049,7 @@
     <t xml:space="preserve">REF.PA.SDH.SDH</t>
   </si>
   <si>
-    <t xml:space="preserve">m2ft</t>
+    <t xml:space="preserve">m2ft, TODO</t>
   </si>
   <si>
     <t xml:space="preserve">020.GBS</t>
@@ -1142,7 +1142,7 @@
     <t xml:space="preserve">not set</t>
   </si>
   <si>
-    <t xml:space="preserve">020.CHN</t>
+    <t xml:space="preserve">custom based on 020.CHN</t>
   </si>
   <si>
     <t xml:space="preserve">custom counter</t>
@@ -1172,16 +1172,19 @@
     <t xml:space="preserve">170.CDM</t>
   </si>
   <si>
+    <t xml:space="preserve">values not described, kept original</t>
+  </si>
+  <si>
     <t xml:space="preserve">170.CST</t>
   </si>
   <si>
     <t xml:space="preserve">170.CNF</t>
   </si>
   <si>
+    <t xml:space="preserve">flag invert</t>
+  </si>
+  <si>
     <t xml:space="preserve">170.TRE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">flag invert</t>
   </si>
   <si>
     <t xml:space="preserve">170.GHO</t>
@@ -1302,7 +1305,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1319,8 +1322,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1347,7 +1362,7 @@
   <dimension ref="A1:U98"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U2" activeCellId="0" sqref="U2"/>
+      <selection pane="topLeft" activeCell="U2" activeCellId="1" sqref="C:E U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3619,24 +3634,24 @@
   </sheetPr>
   <dimension ref="A1:I98"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E99" activeCellId="0" sqref="E99"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E37" activeCellId="0" sqref="C:E"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="53.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50.79"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="2" min="2" style="0" width="50.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="47.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="30.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="53.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.32"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>309</v>
       </c>
@@ -3678,7 +3693,7 @@
       <c r="D2" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>319</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -3689,7 +3704,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>320</v>
       </c>
       <c r="B3" s="0" t="s">
@@ -3801,7 +3816,7 @@
       <c r="D8" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="1" t="s">
         <v>326</v>
       </c>
       <c r="F8" s="1" t="s">
@@ -3868,7 +3883,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
         <v>330</v>
       </c>
@@ -3881,14 +3896,14 @@
       <c r="D12" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="E12" s="1" t="s">
         <v>326</v>
       </c>
       <c r="I12" s="0" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
         <v>331</v>
       </c>
@@ -3901,7 +3916,7 @@
       <c r="D13" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="E13" s="1" t="s">
         <v>332</v>
       </c>
       <c r="I13" s="0" t="s">
@@ -3949,7 +3964,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="4" t="s">
         <v>335</v>
       </c>
       <c r="B16" s="0" t="s">
@@ -3998,7 +4013,7 @@
       <c r="D18" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="6" t="s">
         <v>337</v>
       </c>
       <c r="F18" s="1" t="s">
@@ -4009,7 +4024,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="5" t="s">
         <v>338</v>
       </c>
       <c r="B19" s="0" t="s">
@@ -4021,7 +4036,7 @@
       <c r="D19" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="7" t="s">
         <v>339</v>
       </c>
       <c r="F19" s="1" t="s">
@@ -4118,7 +4133,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="5" t="s">
         <v>341</v>
       </c>
       <c r="B24" s="0" t="s">
@@ -4130,7 +4145,7 @@
       <c r="D24" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="E24" s="0" t="s">
+      <c r="E24" s="7" t="s">
         <v>342</v>
       </c>
       <c r="I24" s="0" t="s">
@@ -4167,7 +4182,7 @@
       <c r="D26" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="E26" s="0" t="s">
+      <c r="E26" s="1" t="s">
         <v>337</v>
       </c>
       <c r="F26" s="1" t="s">
@@ -4190,6 +4205,9 @@
       <c r="D27" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="E27" s="1" t="s">
+        <v>326</v>
+      </c>
       <c r="F27" s="1" t="s">
         <v>95</v>
       </c>
@@ -4218,6 +4236,9 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="4" t="s">
+        <v>333</v>
+      </c>
       <c r="B29" s="0" t="s">
         <v>101</v>
       </c>
@@ -4235,7 +4256,7 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="5" t="s">
         <v>338</v>
       </c>
       <c r="B30" s="0" t="s">
@@ -4247,7 +4268,7 @@
       <c r="D30" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E30" s="7" t="s">
         <v>345</v>
       </c>
       <c r="F30" s="1" t="s">
@@ -4257,7 +4278,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="s">
         <v>107</v>
       </c>
@@ -4267,7 +4288,7 @@
       <c r="D31" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E31" s="7" t="s">
         <v>346</v>
       </c>
       <c r="F31" s="1" t="s">
@@ -4277,7 +4298,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="s">
         <v>110</v>
       </c>
@@ -4287,7 +4308,7 @@
       <c r="D32" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="E32" s="0" t="s">
+      <c r="E32" s="1" t="s">
         <v>347</v>
       </c>
       <c r="F32" s="1" t="s">
@@ -4297,7 +4318,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
         <v>113</v>
       </c>
@@ -4307,7 +4328,7 @@
       <c r="D33" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E33" s="0" t="s">
+      <c r="E33" s="1" t="s">
         <v>347</v>
       </c>
       <c r="F33" s="1" t="s">
@@ -4317,7 +4338,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
         <v>116</v>
       </c>
@@ -4327,7 +4348,7 @@
       <c r="D34" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E34" s="0" t="s">
+      <c r="E34" s="1" t="s">
         <v>347</v>
       </c>
       <c r="F34" s="1" t="s">
@@ -4337,7 +4358,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
         <v>119</v>
       </c>
@@ -4347,7 +4368,7 @@
       <c r="D35" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E35" s="0" t="s">
+      <c r="E35" s="1" t="s">
         <v>347</v>
       </c>
       <c r="F35" s="1" t="s">
@@ -4357,7 +4378,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
         <v>122</v>
       </c>
@@ -4367,7 +4388,7 @@
       <c r="D36" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="E36" s="0" t="s">
+      <c r="E36" s="1" t="s">
         <v>347</v>
       </c>
       <c r="F36" s="1" t="s">
@@ -4377,7 +4398,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
         <v>125</v>
       </c>
@@ -4387,7 +4408,7 @@
       <c r="D37" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E37" s="0" t="s">
+      <c r="E37" s="1" t="s">
         <v>347</v>
       </c>
       <c r="F37" s="1" t="s">
@@ -4397,7 +4418,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
         <v>128</v>
       </c>
@@ -4407,7 +4428,7 @@
       <c r="D38" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E38" s="0" t="s">
+      <c r="E38" s="1" t="s">
         <v>347</v>
       </c>
       <c r="F38" s="1" t="s">
@@ -4417,7 +4438,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="0" t="s">
         <v>131</v>
       </c>
@@ -4427,7 +4448,7 @@
       <c r="D39" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E39" s="0" t="s">
+      <c r="E39" s="1" t="s">
         <v>347</v>
       </c>
       <c r="F39" s="1" t="s">
@@ -4458,7 +4479,7 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="5" t="s">
+      <c r="A41" s="8" t="s">
         <v>349</v>
       </c>
       <c r="B41" s="0" t="s">
@@ -4469,6 +4490,9 @@
       </c>
       <c r="D41" s="0" t="s">
         <v>12</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>326</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>139</v>
@@ -4490,6 +4514,9 @@
       <c r="D42" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="E42" s="1" t="s">
+        <v>326</v>
+      </c>
       <c r="F42" s="1" t="s">
         <v>142</v>
       </c>
@@ -4510,6 +4537,9 @@
       <c r="D43" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="E43" s="1" t="s">
+        <v>332</v>
+      </c>
       <c r="F43" s="1" t="s">
         <v>145</v>
       </c>
@@ -4527,7 +4557,7 @@
       <c r="D44" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="E44" s="0" t="s">
+      <c r="E44" s="1" t="s">
         <v>352</v>
       </c>
       <c r="F44" s="1" t="s">
@@ -4547,7 +4577,7 @@
       <c r="D45" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="E45" s="0" t="s">
+      <c r="E45" s="1" t="s">
         <v>353</v>
       </c>
       <c r="F45" s="1" t="s">
@@ -4597,7 +4627,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="0" t="s">
         <v>159</v>
       </c>
@@ -4607,7 +4637,7 @@
       <c r="D48" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="E48" s="0" t="s">
+      <c r="E48" s="1" t="s">
         <v>352</v>
       </c>
       <c r="I48" s="0" t="s">
@@ -4647,7 +4677,7 @@
       <c r="D50" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="E50" s="0" t="s">
+      <c r="E50" s="1" t="s">
         <v>358</v>
       </c>
       <c r="F50" s="1" t="s">
@@ -4673,7 +4703,7 @@
       <c r="D51" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E51" s="0" t="s">
+      <c r="E51" s="1" t="s">
         <v>359</v>
       </c>
       <c r="F51" s="1" t="s">
@@ -4696,7 +4726,7 @@
       <c r="D52" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="E52" s="0" t="s">
+      <c r="E52" s="1" t="s">
         <v>361</v>
       </c>
       <c r="F52" s="1" t="s">
@@ -4716,7 +4746,7 @@
       <c r="D53" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="0" t="s">
+      <c r="E53" s="1" t="s">
         <v>359</v>
       </c>
       <c r="F53" s="1" t="s">
@@ -4739,7 +4769,7 @@
       <c r="D54" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="E54" s="0" t="s">
+      <c r="E54" s="1" t="s">
         <v>361</v>
       </c>
       <c r="F54" s="1" t="s">
@@ -4759,7 +4789,7 @@
       <c r="D55" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E55" s="0" t="s">
+      <c r="E55" s="1" t="s">
         <v>359</v>
       </c>
       <c r="F55" s="1" t="s">
@@ -4782,7 +4812,7 @@
       <c r="D56" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="E56" s="0" t="s">
+      <c r="E56" s="1" t="s">
         <v>358</v>
       </c>
       <c r="F56" s="1" t="s">
@@ -4808,7 +4838,7 @@
       <c r="D57" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E57" s="0" t="s">
+      <c r="E57" s="1" t="s">
         <v>359</v>
       </c>
       <c r="F57" s="1" t="s">
@@ -4831,6 +4861,9 @@
       <c r="D58" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="E58" s="1" t="s">
+        <v>326</v>
+      </c>
       <c r="F58" s="1" t="s">
         <v>190</v>
       </c>
@@ -4839,7 +4872,7 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="5" t="s">
+      <c r="A59" s="8" t="s">
         <v>365</v>
       </c>
       <c r="B59" s="0" t="s">
@@ -4851,7 +4884,7 @@
       <c r="D59" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="E59" s="0" t="s">
+      <c r="E59" s="1" t="s">
         <v>358</v>
       </c>
       <c r="F59" s="1" t="s">
@@ -4861,7 +4894,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
         <v>366</v>
       </c>
@@ -4874,14 +4907,14 @@
       <c r="D60" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="E60" s="0" t="s">
+      <c r="E60" s="1" t="s">
         <v>358</v>
       </c>
       <c r="I60" s="0" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="0" t="s">
         <v>197</v>
       </c>
@@ -4891,14 +4924,14 @@
       <c r="D61" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="E61" s="4" t="s">
+      <c r="E61" s="7" t="s">
         <v>346</v>
       </c>
       <c r="I61" s="0" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
         <v>367</v>
       </c>
@@ -4911,14 +4944,14 @@
       <c r="D62" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="E62" s="0" t="s">
+      <c r="E62" s="1" t="s">
         <v>368</v>
       </c>
       <c r="I62" s="0" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="0" t="s">
         <v>201</v>
       </c>
@@ -4928,14 +4961,14 @@
       <c r="D63" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="E63" s="4" t="s">
+      <c r="E63" s="7" t="s">
         <v>346</v>
       </c>
       <c r="I63" s="0" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
         <v>369</v>
       </c>
@@ -4948,14 +4981,14 @@
       <c r="D64" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="E64" s="0" t="s">
+      <c r="E64" s="1" t="s">
         <v>368</v>
       </c>
       <c r="I64" s="0" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="0" t="s">
         <v>205</v>
       </c>
@@ -4965,7 +4998,7 @@
       <c r="D65" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="E65" s="4" t="s">
+      <c r="E65" s="7" t="s">
         <v>346</v>
       </c>
       <c r="I65" s="0" t="s">
@@ -5022,7 +5055,7 @@
       <c r="D68" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="E68" s="4" t="s">
+      <c r="E68" s="7" t="s">
         <v>346</v>
       </c>
       <c r="F68" s="1" t="s">
@@ -5042,7 +5075,7 @@
       <c r="D69" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="E69" s="4" t="s">
+      <c r="E69" s="7" t="s">
         <v>346</v>
       </c>
       <c r="F69" s="1" t="s">
@@ -5062,7 +5095,7 @@
       <c r="D70" s="0" t="s">
         <v>220</v>
       </c>
-      <c r="E70" s="0" t="s">
+      <c r="E70" s="1" t="s">
         <v>372</v>
       </c>
       <c r="F70" s="1" t="s">
@@ -5073,7 +5106,7 @@
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
+      <c r="A71" s="5" t="s">
         <v>373</v>
       </c>
       <c r="B71" s="0" t="s">
@@ -5113,7 +5146,7 @@
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="4" t="s">
+      <c r="A73" s="5" t="s">
         <v>338</v>
       </c>
       <c r="B73" s="0" t="s">
@@ -5125,7 +5158,7 @@
       <c r="D73" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="E73" s="4" t="s">
+      <c r="E73" s="7" t="s">
         <v>345</v>
       </c>
       <c r="F73" s="1" t="s">
@@ -5136,7 +5169,7 @@
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="4" t="s">
+      <c r="A74" s="5" t="s">
         <v>338</v>
       </c>
       <c r="B74" s="0" t="s">
@@ -5148,7 +5181,7 @@
       <c r="D74" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="E74" s="4" t="s">
+      <c r="E74" s="7" t="s">
         <v>345</v>
       </c>
       <c r="F74" s="1" t="s">
@@ -5208,7 +5241,7 @@
       <c r="D77" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="E77" s="0" t="s">
+      <c r="E77" s="1" t="s">
         <v>358</v>
       </c>
       <c r="F77" s="1" t="s">
@@ -5231,7 +5264,7 @@
       <c r="D78" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E78" s="0" t="s">
+      <c r="E78" s="1" t="s">
         <v>326</v>
       </c>
       <c r="F78" s="1" t="s">
@@ -5254,7 +5287,7 @@
       <c r="D79" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E79" s="0" t="s">
+      <c r="E79" s="1" t="s">
         <v>326</v>
       </c>
       <c r="F79" s="1" t="s">
@@ -5297,7 +5330,7 @@
       <c r="D81" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E81" s="0" t="s">
+      <c r="E81" s="1" t="s">
         <v>326</v>
       </c>
       <c r="F81" s="1" t="s">
@@ -5363,6 +5396,9 @@
       <c r="D84" s="0" t="s">
         <v>268</v>
       </c>
+      <c r="E84" s="1" t="s">
+        <v>383</v>
+      </c>
       <c r="F84" s="1" t="s">
         <v>269</v>
       </c>
@@ -5372,7 +5408,7 @@
     </row>
     <row r="85" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B85" s="0" t="s">
         <v>271</v>
@@ -5383,7 +5419,7 @@
       <c r="D85" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E85" s="0" t="s">
+      <c r="E85" s="1" t="s">
         <v>326</v>
       </c>
       <c r="F85" s="1" t="s">
@@ -5393,9 +5429,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B86" s="0" t="s">
         <v>274</v>
@@ -5406,8 +5442,8 @@
       <c r="D86" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E86" s="0" t="s">
-        <v>326</v>
+      <c r="E86" s="1" t="s">
+        <v>386</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>275</v>
@@ -5418,7 +5454,7 @@
     </row>
     <row r="87" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="B87" s="0" t="s">
         <v>277</v>
@@ -5430,7 +5466,7 @@
         <v>12</v>
       </c>
       <c r="E87" s="0" t="s">
-        <v>386</v>
+        <v>326</v>
       </c>
       <c r="F87" s="1" t="s">
         <v>278</v>
@@ -5441,7 +5477,7 @@
     </row>
     <row r="88" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B88" s="0" t="s">
         <v>280</v>
@@ -5452,7 +5488,7 @@
       <c r="D88" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E88" s="0" t="s">
+      <c r="E88" s="1" t="s">
         <v>326</v>
       </c>
       <c r="F88" s="1" t="s">
@@ -5464,7 +5500,7 @@
     </row>
     <row r="89" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B89" s="0" t="s">
         <v>283</v>
@@ -5475,7 +5511,7 @@
       <c r="D89" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E89" s="0" t="s">
+      <c r="E89" s="1" t="s">
         <v>326</v>
       </c>
       <c r="F89" s="1" t="s">
@@ -5487,7 +5523,7 @@
     </row>
     <row r="90" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B90" s="0" t="s">
         <v>286</v>
@@ -5505,9 +5541,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B91" s="0" t="s">
         <v>289</v>
@@ -5518,16 +5554,16 @@
       <c r="D91" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E91" s="0" t="s">
+      <c r="E91" s="1" t="s">
         <v>326</v>
       </c>
       <c r="I91" s="0" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B92" s="0" t="s">
         <v>291</v>
@@ -5538,16 +5574,16 @@
       <c r="D92" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E92" s="0" t="s">
+      <c r="E92" s="1" t="s">
         <v>326</v>
       </c>
       <c r="I92" s="0" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B93" s="0" t="s">
         <v>293</v>
@@ -5558,16 +5594,16 @@
       <c r="D93" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E93" s="0" t="s">
+      <c r="E93" s="1" t="s">
         <v>326</v>
       </c>
       <c r="I93" s="0" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B94" s="0" t="s">
         <v>295</v>
@@ -5578,16 +5614,16 @@
       <c r="D94" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E94" s="0" t="s">
+      <c r="E94" s="1" t="s">
         <v>326</v>
       </c>
       <c r="I94" s="0" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B95" s="0" t="s">
         <v>297</v>
@@ -5598,16 +5634,16 @@
       <c r="D95" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E95" s="0" t="s">
+      <c r="E95" s="1" t="s">
         <v>326</v>
       </c>
       <c r="I95" s="0" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B96" s="0" t="s">
         <v>299</v>
@@ -5618,7 +5654,7 @@
       <c r="D96" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E96" s="0" t="s">
+      <c r="E96" s="1" t="s">
         <v>326</v>
       </c>
       <c r="I96" s="0" t="s">
@@ -5627,7 +5663,7 @@
     </row>
     <row r="97" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B97" s="0" t="s">
         <v>301</v>
@@ -5653,7 +5689,7 @@
     </row>
     <row r="98" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B98" s="0" t="s">
         <v>306</v>

</xml_diff>